<commit_message>
inventory change stock automation updated
</commit_message>
<xml_diff>
--- a/resources/Sku/SKU.xlsx
+++ b/resources/Sku/SKU.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B5B4B9-A7B2-4525-8C4A-2E65D10753EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBF02AE-0D17-42F4-B629-52604D1E335F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,10 +94,10 @@
     <t>valueText</t>
   </si>
   <si>
-    <t>test SKU 999</t>
-  </si>
-  <si>
     <t>NoOfSku</t>
+  </si>
+  <si>
+    <t>test SKU 992</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2">
         <v>1</v>
@@ -544,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>